<commit_message>
test: add tests for cell validation with multiple cell validators
</commit_message>
<xml_diff>
--- a/src/test/resources/Fake_Employee_Data.xlsx
+++ b/src/test/resources/Fake_Employee_Data.xlsx
@@ -10,17 +10,17 @@
   <sheets>
     <sheet name="Employee Records" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t xml:space="preserve">Employee ID</t>
   </si>
@@ -40,121 +40,118 @@
     <t xml:space="preserve">Hire Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Jessica Gray</t>
+    <t xml:space="preserve">Benja Rod</t>
   </si>
   <si>
     <t xml:space="preserve">Horticultural consultant</t>
   </si>
   <si>
-    <t xml:space="preserve">Keith Lawrence</t>
+    <t xml:space="preserve">Alexa Oli</t>
   </si>
   <si>
     <t xml:space="preserve">Building services engineer</t>
   </si>
   <si>
-    <t xml:space="preserve">Craig Sanchez</t>
+    <t xml:space="preserve">Patri Mor</t>
   </si>
   <si>
     <t xml:space="preserve">Ceramics designer</t>
   </si>
   <si>
-    <t xml:space="preserve">Timothy Parks</t>
+    <t xml:space="preserve">Chris Joh</t>
   </si>
   <si>
     <t xml:space="preserve">Tax inspector</t>
   </si>
   <si>
-    <t xml:space="preserve">Jennifer White</t>
+    <t xml:space="preserve">Benja Joh</t>
   </si>
   <si>
     <t xml:space="preserve">Chartered management accountant</t>
   </si>
   <si>
-    <t xml:space="preserve">Jessica Schneider</t>
+    <t xml:space="preserve">Jonaa Bro</t>
   </si>
   <si>
     <t xml:space="preserve">Public house manager</t>
   </si>
   <si>
-    <t xml:space="preserve">Jasmine Robbins</t>
+    <t xml:space="preserve">Saman Bro</t>
   </si>
   <si>
     <t xml:space="preserve">Careers adviser</t>
   </si>
   <si>
-    <t xml:space="preserve">Robert Stokes</t>
+    <t xml:space="preserve">Frede Rod</t>
   </si>
   <si>
     <t xml:space="preserve">Surveyor, building control</t>
   </si>
   <si>
-    <t xml:space="preserve">Michael Miller</t>
+    <t xml:space="preserve">Patri Smi</t>
   </si>
   <si>
     <t xml:space="preserve">Newspaper journalist</t>
   </si>
   <si>
-    <t xml:space="preserve">David Griffin</t>
+    <t xml:space="preserve">Saman Joh</t>
   </si>
   <si>
     <t xml:space="preserve">Local government officer</t>
   </si>
   <si>
-    <t xml:space="preserve">Robert Gonzalez</t>
+    <t xml:space="preserve">Charl Smi</t>
   </si>
   <si>
     <t xml:space="preserve">Investment banker, operational</t>
   </si>
   <si>
-    <t xml:space="preserve">Lisa Payne</t>
+    <t xml:space="preserve">Alexa McK</t>
   </si>
   <si>
     <t xml:space="preserve">Hospital doctor</t>
   </si>
   <si>
-    <t xml:space="preserve">Michael Horn</t>
-  </si>
-  <si>
     <t xml:space="preserve">Data processing manager</t>
   </si>
   <si>
-    <t xml:space="preserve">Bruce Parks</t>
+    <t xml:space="preserve">Charl Joh</t>
   </si>
   <si>
     <t xml:space="preserve">Firefighter</t>
   </si>
   <si>
-    <t xml:space="preserve">Dana Wiggins</t>
+    <t xml:space="preserve">Chris Fit</t>
   </si>
   <si>
     <t xml:space="preserve">Set designer</t>
   </si>
   <si>
-    <t xml:space="preserve">Charles Ryan</t>
+    <t xml:space="preserve">Patri Mar</t>
   </si>
   <si>
     <t xml:space="preserve">Occupational psychologist</t>
   </si>
   <si>
-    <t xml:space="preserve">John Dudley</t>
+    <t xml:space="preserve">Frede Mor</t>
   </si>
   <si>
     <t xml:space="preserve">Further education lecturer</t>
   </si>
   <si>
-    <t xml:space="preserve">Peter Esparza</t>
+    <t xml:space="preserve">Benja Mor</t>
   </si>
   <si>
     <t xml:space="preserve">Armed forces technical officer</t>
   </si>
   <si>
-    <t xml:space="preserve">Shannon Clay</t>
+    <t xml:space="preserve">Saman Rod</t>
   </si>
   <si>
     <t xml:space="preserve">Engineer, broadcasting (operations)</t>
   </si>
   <si>
-    <t xml:space="preserve">Brian Holland</t>
+    <t xml:space="preserve">Danie McK</t>
   </si>
   <si>
     <t xml:space="preserve">Financial trader</t>
@@ -166,12 +163,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -190,6 +188,14 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -199,12 +205,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -238,11 +251,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -259,9 +272,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="LibreOffice">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
@@ -269,46 +282,46 @@
         <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="1f497d"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="eeece1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18a303"/>
+        <a:srgbClr val="4f81bd"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369a3"/>
+        <a:srgbClr val="c0504d"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a33e03"/>
+        <a:srgbClr val="9bbb59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8e03a3"/>
+        <a:srgbClr val="8064a2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="c99c00"/>
+        <a:srgbClr val="4bacc6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="c9211e"/>
+        <a:srgbClr val="f79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ee"/>
+        <a:srgbClr val="0000ff"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551a8b"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -316,25 +329,58 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter/>
         </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter/>
         </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -352,12 +398,48 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
@@ -372,20 +454,12 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.81"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -405,400 +479,400 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
         <v>1060</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="0" t="n">
         <v>99574.28</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="0" t="n">
         <v>11</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>36558</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
         <v>8154</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="0" t="n">
         <v>114153.6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="0" t="n">
         <v>31</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>43077</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>6080</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="0" t="n">
         <v>66580.62</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="0" t="n">
         <v>27</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>43152</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
         <v>8924</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="0" t="n">
         <v>103095.63</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="0" t="n">
         <v>10</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>43440</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
         <v>4029</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="0" t="n">
         <v>41845.79</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="0" t="n">
         <v>27</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>37552</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
         <v>6585</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="0" t="n">
         <v>64540.47</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="0" t="n">
         <v>9</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>44462</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
         <v>5681</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="0" t="n">
         <v>102053.19</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="0" t="n">
         <v>39</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>44120</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
         <v>5742</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="0" t="n">
         <v>60651.94</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="0" t="n">
         <v>11</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>44263</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
         <v>6596</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="0" t="n">
         <v>106102.25</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="0" t="n">
         <v>36</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>42073</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
         <v>9294</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="0" t="n">
         <v>45157.63</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="0" t="n">
         <v>30</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>45124</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
         <v>6625</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="0" t="n">
         <v>108033.27</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="0" t="n">
         <v>23</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>45088</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
         <v>4584</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="0" t="n">
         <v>72339.81</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="0" t="n">
         <v>29</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>32132</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
         <v>4876</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>48709.6</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="1" t="n">
-        <v>48709.6</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="0" t="n">
         <v>20</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>34806</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
         <v>7150</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>72279.72</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="1" t="n">
-        <v>72279.72</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="0" t="n">
         <v>8</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>36200</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
         <v>1284</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>110692.06</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1" t="n">
-        <v>110692.06</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="0" t="n">
         <v>25</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>35489</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
         <v>6382</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>101152.36</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="1" t="n">
-        <v>101152.36</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="0" t="n">
         <v>3</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>33484</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
         <v>2034</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>92627.4</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="1" t="n">
-        <v>92627.4</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>32313</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
         <v>3050</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>117626.75</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="1" t="n">
-        <v>117626.75</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="0" t="n">
         <v>4</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>41798</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
         <v>5906</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>45296.81</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="1" t="n">
-        <v>45296.81</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" s="0" t="n">
         <v>33</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>37475</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
         <v>2702</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>74477.92</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="1" t="n">
-        <v>74477.92</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" s="0" t="n">
         <v>36</v>
       </c>
       <c r="F21" s="2" t="n">
@@ -807,11 +881,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>